<commit_message>
2021.01.05 2145PST making all the spreadsheets...
</commit_message>
<xml_diff>
--- a/Spec Data/specpH.2018.08.10.salmontanks.xlsx
+++ b/Spec Data/specpH.2018.08.10.salmontanks.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OALAB\Documents\Spec pH\2018\August 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinerovinski/GIT/NWFSC.MUK_DGNjuvenile.tanks/Spec Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4078D53-726F-424D-99F0-DC0746A1E145}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="929" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12300" tabRatio="929" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID categories" sheetId="50" r:id="rId1"/>
@@ -46,19 +47,30 @@
     <definedName name="dyeCor_int">#REF!</definedName>
     <definedName name="dyeCor_slope">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shallin Busch</author>
     <author>Maher, Michael</author>
     <author>OA Lab</author>
   </authors>
   <commentList>
-    <comment ref="Y2" authorId="0" shapeId="0">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
+    <comment ref="G3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -140,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1" shapeId="0">
+    <comment ref="J3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="2" shapeId="0">
+    <comment ref="K3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="1" shapeId="0">
+    <comment ref="G4" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -213,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="1" shapeId="0">
+    <comment ref="J4" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -237,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="1" shapeId="0">
+    <comment ref="G5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -262,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="1" shapeId="0">
+    <comment ref="J5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0">
+    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -311,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="1" shapeId="0">
+    <comment ref="G7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -369,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="1" shapeId="0">
+    <comment ref="J7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -393,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="1" shapeId="0">
+    <comment ref="G8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="1" shapeId="0">
+    <comment ref="J8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -602,7 +614,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
@@ -826,8 +838,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1231,16 +1243,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
@@ -1257,7 +1269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="11" t="s">
         <v>29</v>
       </c>
@@ -1285,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1296,7 +1308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1304,17 +1316,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C8">
         <v>7</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C9">
         <v>8</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C10">
         <v>9</v>
       </c>
@@ -1344,7 +1356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11">
         <v>10</v>
       </c>
@@ -1352,7 +1364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C12">
         <v>11</v>
       </c>
@@ -1360,32 +1372,32 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C18" t="s">
         <v>46</v>
       </c>
@@ -1398,21 +1410,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1441,7 +1453,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1488,19 +1500,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1529,7 +1541,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1575,21 +1587,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1664,21 +1676,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1707,7 +1719,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1753,21 +1765,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1796,7 +1808,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1842,19 +1854,19 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1883,7 +1895,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -1929,21 +1941,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -1972,7 +1984,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -2018,21 +2030,21 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -2061,7 +2073,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -2107,21 +2119,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -2150,7 +2162,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -2196,21 +2208,21 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -2239,7 +2251,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -2285,38 +2297,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="7" style="18" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="18" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="18" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" style="18" customWidth="1"/>
     <col min="12" max="12" width="19" style="18" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="18" customWidth="1"/>
-    <col min="14" max="19" width="8.85546875" style="18" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="18" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="18"/>
-    <col min="22" max="24" width="16.28515625" style="18" customWidth="1"/>
-    <col min="25" max="26" width="8.85546875" style="18" customWidth="1"/>
-    <col min="27" max="27" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.85546875" style="18"/>
+    <col min="13" max="13" width="23.5" style="18" customWidth="1"/>
+    <col min="14" max="19" width="8.83203125" style="18" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" style="18" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="18"/>
+    <col min="22" max="24" width="16.33203125" style="18" customWidth="1"/>
+    <col min="25" max="26" width="8.83203125" style="18" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -2342,7 +2354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="24" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="20" t="s">
         <v>23</v>
       </c>
@@ -2426,7 +2438,7 @@
       </c>
       <c r="AB2" s="27"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="15">
         <v>3</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>-5.000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="29" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="15">
         <v>8</v>
       </c>
@@ -2602,7 +2614,7 @@
         <v>-7.9999999999999988E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5" s="15">
         <v>14</v>
       </c>
@@ -2690,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>15</v>
       </c>
@@ -2777,7 +2789,7 @@
         <v>-3.0000000000000027E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>19</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>-4.9999999999999975E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>20</v>
       </c>
@@ -2960,43 +2972,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$D$1:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$E$1:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$B$2:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$C$2:$C$16</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$D$8:$D$14</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'ID categories'!$E$8:$E$14</xm:f>
           </x14:formula1>
@@ -3009,19 +3021,19 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3050,7 +3062,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3096,21 +3108,21 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3139,7 +3151,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3185,19 +3197,19 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3226,7 +3238,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3272,19 +3284,19 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3313,7 +3325,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3359,19 +3371,19 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3446,19 +3458,19 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3487,7 +3499,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3533,19 +3545,19 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3574,7 +3586,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3620,21 +3632,21 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3663,7 +3675,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3709,21 +3721,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3798,21 +3810,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3841,7 +3853,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3879,10 +3891,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="8:16" x14ac:dyDescent="0.15">
       <c r="P5" s="9"/>
     </row>
-    <row r="7" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="8:16" x14ac:dyDescent="0.15">
       <c r="P7" s="9"/>
     </row>
   </sheetData>
@@ -3894,24 +3906,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.15">
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -3940,7 +3952,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -3987,21 +3999,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -4077,19 +4089,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -4118,7 +4130,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -4156,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H11" s="8"/>
     </row>
   </sheetData>
@@ -4168,21 +4180,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -4211,7 +4223,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -4258,21 +4270,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -4301,7 +4313,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>
@@ -4348,21 +4360,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H2" s="2">
         <v>434</v>
       </c>
@@ -4391,7 +4403,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="3" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="8:16" x14ac:dyDescent="0.15">
       <c r="H3" s="5">
         <f>B252</f>
         <v>0</v>

</xml_diff>